<commit_message>
error rectified for all routes
</commit_message>
<xml_diff>
--- a/public/export.xlsx
+++ b/public/export.xlsx
@@ -397,7 +397,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -458,9 +458,37 @@
         <v>emmanuel olajumoke</v>
       </c>
     </row>
+    <row r="5">
+      <c r="A5" t="str">
+        <v>Pepper-Rice with Chicken</v>
+      </c>
+      <c r="B5" t="str">
+        <v>kilimanjaro</v>
+      </c>
+      <c r="C5" t="str">
+        <v>coca-cola</v>
+      </c>
+      <c r="D5" t="str">
+        <v>emmanuel olajumoke</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="str">
+        <v>Pepper-Rice with Chicken</v>
+      </c>
+      <c r="B6" t="str">
+        <v>kilimanjaro</v>
+      </c>
+      <c r="C6" t="str">
+        <v>coca-cola</v>
+      </c>
+      <c r="D6" t="str">
+        <v>emmanuel olajumoke</v>
+      </c>
+    </row>
   </sheetData>
   <ignoredErrors>
-    <ignoredError numberStoredAsText="1" sqref="A1:D4"/>
+    <ignoredError numberStoredAsText="1" sqref="A1:D6"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>